<commit_message>
Errors fixed in the solve Loop Calculation, and ratios solved
</commit_message>
<xml_diff>
--- a/PropionateOxidation.xlsx
+++ b/PropionateOxidation.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" updateLinks="always"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92997D47-C8A0-4178-9930-6B7C2439CAEF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB40F651-4247-4FEA-BE0F-AEDEAB30D0AA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{B1DDE01B-6290-4C58-94E8-4710908F5800}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{B1DDE01B-6290-4C58-94E8-4710908F5800}"/>
   </bookViews>
   <sheets>
     <sheet name="ProDegPaths" sheetId="12" r:id="rId1"/>
@@ -23092,8 +23092,8 @@
   </sheetPr>
   <dimension ref="A1:CU144"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AI24" sqref="AI24"/>
+    <sheetView tabSelected="1" topLeftCell="AE11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AR33" sqref="AR33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -39735,41 +39735,41 @@
       </c>
       <c r="BA77" s="557"/>
       <c r="BB77" s="295"/>
-      <c r="BD77" s="558">
-        <f t="shared" ref="BD77:BL77" si="32">+SUMPRODUCT($BU$25:$BU$65,BD$25:BD$65)</f>
-        <v>0</v>
-      </c>
-      <c r="BE77" s="547">
-        <f t="shared" si="32"/>
-        <v>0</v>
-      </c>
-      <c r="BF77" s="547">
-        <f t="shared" si="32"/>
-        <v>0</v>
-      </c>
-      <c r="BG77" s="547">
-        <f t="shared" si="32"/>
-        <v>-4.16</v>
-      </c>
-      <c r="BH77" s="547">
-        <f t="shared" si="32"/>
-        <v>0</v>
-      </c>
-      <c r="BI77" s="559">
-        <f t="shared" si="32"/>
-        <v>0</v>
-      </c>
-      <c r="BJ77" s="559">
-        <f t="shared" si="32"/>
-        <v>0</v>
-      </c>
-      <c r="BK77" s="559">
-        <f t="shared" si="32"/>
-        <v>7.9600000000000364</v>
-      </c>
-      <c r="BL77" s="559">
-        <f t="shared" si="32"/>
-        <v>4.16</v>
+      <c r="BD77" s="580">
+        <f>+SUMPRODUCT(ProDegPaths!$BX$25:$BX$65,BD$25:BD$65)</f>
+        <v>0</v>
+      </c>
+      <c r="BE77" s="581">
+        <f>+SUMPRODUCT(ProDegPaths!$BX$25:$BX$65,BE$25:BE$65)</f>
+        <v>0</v>
+      </c>
+      <c r="BF77" s="581">
+        <f>+SUMPRODUCT(ProDegPaths!$BX$25:$BX$65,BF$25:BF$65)</f>
+        <v>0</v>
+      </c>
+      <c r="BG77" s="581">
+        <f>+SUMPRODUCT(ProDegPaths!$BX$25:$BX$65,BG$25:BG$65)</f>
+        <v>0</v>
+      </c>
+      <c r="BH77" s="581">
+        <f>+SUMPRODUCT(ProDegPaths!$BX$25:$BX$65,BH$25:BH$65)</f>
+        <v>0</v>
+      </c>
+      <c r="BI77" s="582">
+        <f>+SUMPRODUCT(ProDegPaths!$BX$25:$BX$65,BI$25:BI$65)</f>
+        <v>0</v>
+      </c>
+      <c r="BJ77" s="582">
+        <f>+SUMPRODUCT(ProDegPaths!$BX$25:$BX$65,BJ$25:BJ$65)</f>
+        <v>0</v>
+      </c>
+      <c r="BK77" s="582">
+        <f>+SUMPRODUCT(ProDegPaths!$BX$25:$BX$65,BK$25:BK$65)</f>
+        <v>0</v>
+      </c>
+      <c r="BL77" s="582">
+        <f>+SUMPRODUCT(ProDegPaths!$BX$25:$BX$65,BL$25:BL$65)</f>
+        <v>0</v>
       </c>
       <c r="BM77" s="560"/>
       <c r="BN77" s="295"/>
@@ -39920,40 +39920,40 @@
       </c>
       <c r="BA78" s="415"/>
       <c r="BB78" s="295"/>
-      <c r="BD78" s="580">
-        <f>+SUMPRODUCT(ProDegPaths!$BX$25:$BX$65,BD$25:BD$65)</f>
-        <v>0</v>
-      </c>
-      <c r="BE78" s="581">
-        <f>+SUMPRODUCT(ProDegPaths!$BX$25:$BX$65,BE$25:BE$65)</f>
-        <v>0</v>
-      </c>
-      <c r="BF78" s="581">
-        <f>+SUMPRODUCT(ProDegPaths!$BX$25:$BX$65,BF$25:BF$65)</f>
-        <v>0</v>
-      </c>
-      <c r="BG78" s="581">
-        <f>+SUMPRODUCT(ProDegPaths!$BX$25:$BX$65,BG$25:BG$65)</f>
-        <v>0</v>
-      </c>
-      <c r="BH78" s="581">
-        <f>+SUMPRODUCT(ProDegPaths!$BX$25:$BX$65,BH$25:BH$65)</f>
-        <v>0</v>
-      </c>
-      <c r="BI78" s="582">
-        <f>+SUMPRODUCT(ProDegPaths!$BX$25:$BX$65,BI$25:BI$65)</f>
-        <v>0</v>
-      </c>
-      <c r="BJ78" s="582">
-        <f>+SUMPRODUCT(ProDegPaths!$BX$25:$BX$65,BJ$25:BJ$65)</f>
-        <v>0</v>
-      </c>
-      <c r="BK78" s="582">
-        <f>+SUMPRODUCT(ProDegPaths!$BX$25:$BX$65,BK$25:BK$65)</f>
-        <v>0</v>
-      </c>
-      <c r="BL78" s="582">
-        <f>+SUMPRODUCT(ProDegPaths!$BX$25:$BX$65,BL$25:BL$65)</f>
+      <c r="BD78" s="587">
+        <f>+SUMPRODUCT(ProDegPaths!$BY$25:$BY$65,BD$25:BD$65)</f>
+        <v>0</v>
+      </c>
+      <c r="BE78" s="588">
+        <f>+SUMPRODUCT(ProDegPaths!$BY$25:$BY$65,BE$25:BE$65)</f>
+        <v>0</v>
+      </c>
+      <c r="BF78" s="588">
+        <f>+SUMPRODUCT(ProDegPaths!$BY$25:$BY$65,BF$25:BF$65)</f>
+        <v>0</v>
+      </c>
+      <c r="BG78" s="588">
+        <f>+SUMPRODUCT(ProDegPaths!$BY$25:$BY$65,BG$25:BG$65)</f>
+        <v>0</v>
+      </c>
+      <c r="BH78" s="588">
+        <f>+SUMPRODUCT(ProDegPaths!$BY$25:$BY$65,BH$25:BH$65)</f>
+        <v>0</v>
+      </c>
+      <c r="BI78" s="589">
+        <f>+SUMPRODUCT(ProDegPaths!$BY$25:$BY$65,BI$25:BI$65)</f>
+        <v>0</v>
+      </c>
+      <c r="BJ78" s="589">
+        <f>+SUMPRODUCT(ProDegPaths!$BY$25:$BY$65,BJ$25:BJ$65)</f>
+        <v>0</v>
+      </c>
+      <c r="BK78" s="589">
+        <f>+SUMPRODUCT(ProDegPaths!$BY$25:$BY$65,BK$25:BK$65)</f>
+        <v>0</v>
+      </c>
+      <c r="BL78" s="589">
+        <f>+SUMPRODUCT(ProDegPaths!$BY$25:$BY$65,BL$25:BL$65)</f>
         <v>0</v>
       </c>
       <c r="BM78" s="301"/>
@@ -40112,39 +40112,39 @@
       <c r="BA79" s="415"/>
       <c r="BB79" s="295"/>
       <c r="BD79" s="587">
-        <f>+SUMPRODUCT(ProDegPaths!$BY$25:$BY$65,BD$25:BD$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$BZ$25:$BZ$65,BD$25:BD$65)</f>
         <v>0</v>
       </c>
       <c r="BE79" s="588">
-        <f>+SUMPRODUCT(ProDegPaths!$BY$25:$BY$65,BE$25:BE$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$BZ$25:$BZ$65,BE$25:BE$65)</f>
         <v>0</v>
       </c>
       <c r="BF79" s="588">
-        <f>+SUMPRODUCT(ProDegPaths!$BY$25:$BY$65,BF$25:BF$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$BZ$25:$BZ$65,BF$25:BF$65)</f>
         <v>0</v>
       </c>
       <c r="BG79" s="588">
-        <f>+SUMPRODUCT(ProDegPaths!$BY$25:$BY$65,BG$25:BG$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$BZ$25:$BZ$65,BG$25:BG$65)</f>
         <v>0</v>
       </c>
       <c r="BH79" s="588">
-        <f>+SUMPRODUCT(ProDegPaths!$BY$25:$BY$65,BH$25:BH$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$BZ$25:$BZ$65,BH$25:BH$65)</f>
         <v>0</v>
       </c>
       <c r="BI79" s="589">
-        <f>+SUMPRODUCT(ProDegPaths!$BY$25:$BY$65,BI$25:BI$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$BZ$25:$BZ$65,BI$25:BI$65)</f>
         <v>0</v>
       </c>
       <c r="BJ79" s="589">
-        <f>+SUMPRODUCT(ProDegPaths!$BY$25:$BY$65,BJ$25:BJ$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$BZ$25:$BZ$65,BJ$25:BJ$65)</f>
         <v>0</v>
       </c>
       <c r="BK79" s="589">
-        <f>+SUMPRODUCT(ProDegPaths!$BY$25:$BY$65,BK$25:BK$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$BZ$25:$BZ$65,BK$25:BK$65)</f>
         <v>0</v>
       </c>
       <c r="BL79" s="589">
-        <f>+SUMPRODUCT(ProDegPaths!$BY$25:$BY$65,BL$25:BL$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$BZ$25:$BZ$65,BL$25:BL$65)</f>
         <v>0</v>
       </c>
       <c r="BM79" s="301"/>
@@ -40163,7 +40163,7 @@
         <v>3</v>
       </c>
       <c r="N80" s="591">
-        <f t="shared" ref="N80:N86" si="33">+M80/L80</f>
+        <f t="shared" ref="N80:N86" si="32">+M80/L80</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="O80" s="302">
@@ -40309,39 +40309,39 @@
       <c r="BA80" s="415"/>
       <c r="BB80" s="295"/>
       <c r="BD80" s="587">
-        <f>+SUMPRODUCT(ProDegPaths!$BZ$25:$BZ$65,BD$25:BD$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CA$25:$CA$65,BD$25:BD$65)</f>
         <v>0</v>
       </c>
       <c r="BE80" s="588">
-        <f>+SUMPRODUCT(ProDegPaths!$BZ$25:$BZ$65,BE$25:BE$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CA$25:$CA$65,BE$25:BE$65)</f>
         <v>0</v>
       </c>
       <c r="BF80" s="588">
-        <f>+SUMPRODUCT(ProDegPaths!$BZ$25:$BZ$65,BF$25:BF$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CA$25:$CA$65,BF$25:BF$65)</f>
         <v>0</v>
       </c>
       <c r="BG80" s="588">
-        <f>+SUMPRODUCT(ProDegPaths!$BZ$25:$BZ$65,BG$25:BG$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CA$25:$CA$65,BG$25:BG$65)</f>
         <v>0</v>
       </c>
       <c r="BH80" s="588">
-        <f>+SUMPRODUCT(ProDegPaths!$BZ$25:$BZ$65,BH$25:BH$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CA$25:$CA$65,BH$25:BH$65)</f>
         <v>0</v>
       </c>
       <c r="BI80" s="589">
-        <f>+SUMPRODUCT(ProDegPaths!$BZ$25:$BZ$65,BI$25:BI$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CA$25:$CA$65,BI$25:BI$65)</f>
         <v>0</v>
       </c>
       <c r="BJ80" s="589">
-        <f>+SUMPRODUCT(ProDegPaths!$BZ$25:$BZ$65,BJ$25:BJ$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CA$25:$CA$65,BJ$25:BJ$65)</f>
         <v>0</v>
       </c>
       <c r="BK80" s="589">
-        <f>+SUMPRODUCT(ProDegPaths!$BZ$25:$BZ$65,BK$25:BK$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CA$25:$CA$65,BK$25:BK$65)</f>
         <v>0</v>
       </c>
       <c r="BL80" s="589">
-        <f>+SUMPRODUCT(ProDegPaths!$BZ$25:$BZ$65,BL$25:BL$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CA$25:$CA$65,BL$25:BL$65)</f>
         <v>0</v>
       </c>
       <c r="BM80" s="301"/>
@@ -40354,26 +40354,26 @@
       <c r="G81" s="590"/>
       <c r="H81" s="593"/>
       <c r="L81" s="594">
-        <f t="shared" ref="L81:L86" si="34">+L80+1</f>
+        <f t="shared" ref="L81:L86" si="33">+L80+1</f>
         <v>10</v>
       </c>
       <c r="M81" s="301">
         <v>3</v>
       </c>
       <c r="N81" s="591">
-        <f t="shared" si="33"/>
+        <f t="shared" si="32"/>
         <v>0.3</v>
       </c>
       <c r="O81" s="302">
-        <f t="shared" ref="O81:O86" si="35">+N81*$O$78</f>
+        <f t="shared" ref="O81:O86" si="34">+N81*$O$78</f>
         <v>21</v>
       </c>
       <c r="P81" s="302">
-        <f t="shared" ref="P81:Q86" si="36">+$N81*P$78</f>
+        <f t="shared" ref="P81:Q86" si="35">+$N81*P$78</f>
         <v>18</v>
       </c>
       <c r="Q81" s="592">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>15</v>
       </c>
       <c r="S81" s="624" t="s">
@@ -40507,39 +40507,39 @@
       <c r="BA81" s="415"/>
       <c r="BB81" s="295"/>
       <c r="BD81" s="587">
-        <f>+SUMPRODUCT(ProDegPaths!$CA$25:$CA$65,BD$25:BD$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CB$25:$CB$65,BD$25:BD$65)</f>
         <v>0</v>
       </c>
       <c r="BE81" s="588">
-        <f>+SUMPRODUCT(ProDegPaths!$CA$25:$CA$65,BE$25:BE$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CB$25:$CB$65,BE$25:BE$65)</f>
         <v>0</v>
       </c>
       <c r="BF81" s="588">
-        <f>+SUMPRODUCT(ProDegPaths!$CA$25:$CA$65,BF$25:BF$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CB$25:$CB$65,BF$25:BF$65)</f>
         <v>0</v>
       </c>
       <c r="BG81" s="588">
-        <f>+SUMPRODUCT(ProDegPaths!$CA$25:$CA$65,BG$25:BG$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CB$25:$CB$65,BG$25:BG$65)</f>
         <v>0</v>
       </c>
       <c r="BH81" s="588">
-        <f>+SUMPRODUCT(ProDegPaths!$CA$25:$CA$65,BH$25:BH$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CB$25:$CB$65,BH$25:BH$65)</f>
         <v>0</v>
       </c>
       <c r="BI81" s="589">
-        <f>+SUMPRODUCT(ProDegPaths!$CA$25:$CA$65,BI$25:BI$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CB$25:$CB$65,BI$25:BI$65)</f>
         <v>0</v>
       </c>
       <c r="BJ81" s="589">
-        <f>+SUMPRODUCT(ProDegPaths!$CA$25:$CA$65,BJ$25:BJ$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CB$25:$CB$65,BJ$25:BJ$65)</f>
         <v>0</v>
       </c>
       <c r="BK81" s="589">
-        <f>+SUMPRODUCT(ProDegPaths!$CA$25:$CA$65,BK$25:BK$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CB$25:$CB$65,BK$25:BK$65)</f>
         <v>0</v>
       </c>
       <c r="BL81" s="589">
-        <f>+SUMPRODUCT(ProDegPaths!$CA$25:$CA$65,BL$25:BL$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CB$25:$CB$65,BL$25:BL$65)</f>
         <v>0</v>
       </c>
       <c r="BM81" s="301"/>
@@ -40552,26 +40552,26 @@
       <c r="G82" s="590"/>
       <c r="H82" s="595"/>
       <c r="L82" s="594">
-        <f t="shared" si="34"/>
+        <f t="shared" si="33"/>
         <v>11</v>
       </c>
       <c r="M82" s="301">
         <v>3</v>
       </c>
       <c r="N82" s="591">
-        <f t="shared" si="33"/>
+        <f t="shared" si="32"/>
         <v>0.27272727272727271</v>
       </c>
       <c r="O82" s="302">
+        <f t="shared" si="34"/>
+        <v>19.09090909090909</v>
+      </c>
+      <c r="P82" s="302">
         <f t="shared" si="35"/>
-        <v>19.09090909090909</v>
-      </c>
-      <c r="P82" s="302">
-        <f t="shared" si="36"/>
         <v>16.363636363636363</v>
       </c>
       <c r="Q82" s="592">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>13.636363636363635</v>
       </c>
       <c r="S82" s="624" t="s">
@@ -40705,39 +40705,39 @@
       <c r="BA82" s="415"/>
       <c r="BB82" s="295"/>
       <c r="BD82" s="587">
-        <f>+SUMPRODUCT(ProDegPaths!$CB$25:$CB$65,BD$25:BD$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CC$25:$CC$65,BD$25:BD$65)</f>
         <v>0</v>
       </c>
       <c r="BE82" s="588">
-        <f>+SUMPRODUCT(ProDegPaths!$CB$25:$CB$65,BE$25:BE$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CC$25:$CC$65,BE$25:BE$65)</f>
         <v>0</v>
       </c>
       <c r="BF82" s="588">
-        <f>+SUMPRODUCT(ProDegPaths!$CB$25:$CB$65,BF$25:BF$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CC$25:$CC$65,BF$25:BF$65)</f>
         <v>0</v>
       </c>
       <c r="BG82" s="588">
-        <f>+SUMPRODUCT(ProDegPaths!$CB$25:$CB$65,BG$25:BG$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CC$25:$CC$65,BG$25:BG$65)</f>
         <v>0</v>
       </c>
       <c r="BH82" s="588">
-        <f>+SUMPRODUCT(ProDegPaths!$CB$25:$CB$65,BH$25:BH$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CC$25:$CC$65,BH$25:BH$65)</f>
         <v>0</v>
       </c>
       <c r="BI82" s="589">
-        <f>+SUMPRODUCT(ProDegPaths!$CB$25:$CB$65,BI$25:BI$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CC$25:$CC$65,BI$25:BI$65)</f>
         <v>0</v>
       </c>
       <c r="BJ82" s="589">
-        <f>+SUMPRODUCT(ProDegPaths!$CB$25:$CB$65,BJ$25:BJ$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CC$25:$CC$65,BJ$25:BJ$65)</f>
         <v>0</v>
       </c>
       <c r="BK82" s="589">
-        <f>+SUMPRODUCT(ProDegPaths!$CB$25:$CB$65,BK$25:BK$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CC$25:$CC$65,BK$25:BK$65)</f>
         <v>0</v>
       </c>
       <c r="BL82" s="589">
-        <f>+SUMPRODUCT(ProDegPaths!$CB$25:$CB$65,BL$25:BL$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CC$25:$CC$65,BL$25:BL$65)</f>
         <v>0</v>
       </c>
       <c r="BM82" s="301"/>
@@ -40750,26 +40750,26 @@
       <c r="G83" s="590"/>
       <c r="H83" s="595"/>
       <c r="L83" s="594">
-        <f t="shared" si="34"/>
+        <f t="shared" si="33"/>
         <v>12</v>
       </c>
       <c r="M83" s="301">
         <v>3</v>
       </c>
       <c r="N83" s="591">
-        <f t="shared" si="33"/>
+        <f t="shared" si="32"/>
         <v>0.25</v>
       </c>
       <c r="O83" s="302">
+        <f t="shared" si="34"/>
+        <v>17.5</v>
+      </c>
+      <c r="P83" s="302">
         <f t="shared" si="35"/>
-        <v>17.5</v>
-      </c>
-      <c r="P83" s="302">
-        <f t="shared" si="36"/>
         <v>15</v>
       </c>
       <c r="Q83" s="592">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>12.5</v>
       </c>
       <c r="S83" s="624" t="s">
@@ -40903,39 +40903,39 @@
       <c r="BA83" s="415"/>
       <c r="BB83" s="295"/>
       <c r="BD83" s="587">
-        <f>+SUMPRODUCT(ProDegPaths!$CC$25:$CC$65,BD$25:BD$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CD$25:$CD$65,BD$25:BD$65)</f>
         <v>0</v>
       </c>
       <c r="BE83" s="588">
-        <f>+SUMPRODUCT(ProDegPaths!$CC$25:$CC$65,BE$25:BE$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CD$25:$CD$65,BE$25:BE$65)</f>
         <v>0</v>
       </c>
       <c r="BF83" s="588">
-        <f>+SUMPRODUCT(ProDegPaths!$CC$25:$CC$65,BF$25:BF$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CD$25:$CD$65,BF$25:BF$65)</f>
         <v>0</v>
       </c>
       <c r="BG83" s="588">
-        <f>+SUMPRODUCT(ProDegPaths!$CC$25:$CC$65,BG$25:BG$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CD$25:$CD$65,BG$25:BG$65)</f>
         <v>0</v>
       </c>
       <c r="BH83" s="588">
-        <f>+SUMPRODUCT(ProDegPaths!$CC$25:$CC$65,BH$25:BH$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CD$25:$CD$65,BH$25:BH$65)</f>
         <v>0</v>
       </c>
       <c r="BI83" s="589">
-        <f>+SUMPRODUCT(ProDegPaths!$CC$25:$CC$65,BI$25:BI$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CD$25:$CD$65,BI$25:BI$65)</f>
         <v>0</v>
       </c>
       <c r="BJ83" s="589">
-        <f>+SUMPRODUCT(ProDegPaths!$CC$25:$CC$65,BJ$25:BJ$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CD$25:$CD$65,BJ$25:BJ$65)</f>
         <v>0</v>
       </c>
       <c r="BK83" s="589">
-        <f>+SUMPRODUCT(ProDegPaths!$CC$25:$CC$65,BK$25:BK$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CD$25:$CD$65,BK$25:BK$65)</f>
         <v>0</v>
       </c>
       <c r="BL83" s="589">
-        <f>+SUMPRODUCT(ProDegPaths!$CC$25:$CC$65,BL$25:BL$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CD$25:$CD$65,BL$25:BL$65)</f>
         <v>0</v>
       </c>
       <c r="BM83" s="301"/>
@@ -40948,26 +40948,26 @@
       <c r="G84" s="590"/>
       <c r="H84" s="595"/>
       <c r="L84" s="594">
-        <f t="shared" si="34"/>
+        <f t="shared" si="33"/>
         <v>13</v>
       </c>
       <c r="M84" s="301">
         <v>3</v>
       </c>
       <c r="N84" s="591">
-        <f t="shared" si="33"/>
+        <f t="shared" si="32"/>
         <v>0.23076923076923078</v>
       </c>
       <c r="O84" s="302">
+        <f t="shared" si="34"/>
+        <v>16.153846153846153</v>
+      </c>
+      <c r="P84" s="302">
         <f t="shared" si="35"/>
-        <v>16.153846153846153</v>
-      </c>
-      <c r="P84" s="302">
-        <f t="shared" si="36"/>
         <v>13.846153846153847</v>
       </c>
       <c r="Q84" s="592">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>11.538461538461538</v>
       </c>
       <c r="S84" s="624" t="s">
@@ -41101,39 +41101,39 @@
       <c r="BA84" s="415"/>
       <c r="BB84" s="295"/>
       <c r="BD84" s="587">
-        <f>+SUMPRODUCT(ProDegPaths!$CD$25:$CD$65,BD$25:BD$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CE$25:$CE$65,BD$25:BD$65)</f>
         <v>0</v>
       </c>
       <c r="BE84" s="588">
-        <f>+SUMPRODUCT(ProDegPaths!$CD$25:$CD$65,BE$25:BE$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CE$25:$CE$65,BE$25:BE$65)</f>
         <v>0</v>
       </c>
       <c r="BF84" s="588">
-        <f>+SUMPRODUCT(ProDegPaths!$CD$25:$CD$65,BF$25:BF$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CE$25:$CE$65,BF$25:BF$65)</f>
         <v>0</v>
       </c>
       <c r="BG84" s="588">
-        <f>+SUMPRODUCT(ProDegPaths!$CD$25:$CD$65,BG$25:BG$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CE$25:$CE$65,BG$25:BG$65)</f>
         <v>0</v>
       </c>
       <c r="BH84" s="588">
-        <f>+SUMPRODUCT(ProDegPaths!$CD$25:$CD$65,BH$25:BH$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CE$25:$CE$65,BH$25:BH$65)</f>
         <v>0</v>
       </c>
       <c r="BI84" s="589">
-        <f>+SUMPRODUCT(ProDegPaths!$CD$25:$CD$65,BI$25:BI$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CE$25:$CE$65,BI$25:BI$65)</f>
         <v>0</v>
       </c>
       <c r="BJ84" s="589">
-        <f>+SUMPRODUCT(ProDegPaths!$CD$25:$CD$65,BJ$25:BJ$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CE$25:$CE$65,BJ$25:BJ$65)</f>
         <v>0</v>
       </c>
       <c r="BK84" s="589">
-        <f>+SUMPRODUCT(ProDegPaths!$CD$25:$CD$65,BK$25:BK$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CE$25:$CE$65,BK$25:BK$65)</f>
         <v>0</v>
       </c>
       <c r="BL84" s="589">
-        <f>+SUMPRODUCT(ProDegPaths!$CD$25:$CD$65,BL$25:BL$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CE$25:$CE$65,BL$25:BL$65)</f>
         <v>0</v>
       </c>
       <c r="BM84" s="301"/>
@@ -41146,26 +41146,26 @@
       <c r="G85" s="590"/>
       <c r="H85" s="595"/>
       <c r="L85" s="594">
-        <f t="shared" si="34"/>
+        <f t="shared" si="33"/>
         <v>14</v>
       </c>
       <c r="M85" s="301">
         <v>3</v>
       </c>
       <c r="N85" s="591">
-        <f t="shared" si="33"/>
+        <f t="shared" si="32"/>
         <v>0.21428571428571427</v>
       </c>
       <c r="O85" s="302">
+        <f t="shared" si="34"/>
+        <v>15</v>
+      </c>
+      <c r="P85" s="302">
         <f t="shared" si="35"/>
-        <v>15</v>
-      </c>
-      <c r="P85" s="302">
-        <f t="shared" si="36"/>
         <v>12.857142857142856</v>
       </c>
       <c r="Q85" s="592">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>10.714285714285714</v>
       </c>
       <c r="S85" s="624" t="s">
@@ -41299,39 +41299,39 @@
       <c r="BA85" s="415"/>
       <c r="BB85" s="295"/>
       <c r="BD85" s="587">
-        <f>+SUMPRODUCT(ProDegPaths!$CE$25:$CE$65,BD$25:BD$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CF$25:$CF$65,BD$25:BD$65)</f>
         <v>0</v>
       </c>
       <c r="BE85" s="588">
-        <f>+SUMPRODUCT(ProDegPaths!$CE$25:$CE$65,BE$25:BE$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CF$25:$CF$65,BE$25:BE$65)</f>
         <v>0</v>
       </c>
       <c r="BF85" s="588">
-        <f>+SUMPRODUCT(ProDegPaths!$CE$25:$CE$65,BF$25:BF$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CF$25:$CF$65,BF$25:BF$65)</f>
         <v>0</v>
       </c>
       <c r="BG85" s="588">
-        <f>+SUMPRODUCT(ProDegPaths!$CE$25:$CE$65,BG$25:BG$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CF$25:$CF$65,BG$25:BG$65)</f>
         <v>0</v>
       </c>
       <c r="BH85" s="588">
-        <f>+SUMPRODUCT(ProDegPaths!$CE$25:$CE$65,BH$25:BH$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CF$25:$CF$65,BH$25:BH$65)</f>
         <v>0</v>
       </c>
       <c r="BI85" s="589">
-        <f>+SUMPRODUCT(ProDegPaths!$CE$25:$CE$65,BI$25:BI$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CF$25:$CF$65,BI$25:BI$65)</f>
         <v>0</v>
       </c>
       <c r="BJ85" s="589">
-        <f>+SUMPRODUCT(ProDegPaths!$CE$25:$CE$65,BJ$25:BJ$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CF$25:$CF$65,BJ$25:BJ$65)</f>
         <v>0</v>
       </c>
       <c r="BK85" s="589">
-        <f>+SUMPRODUCT(ProDegPaths!$CE$25:$CE$65,BK$25:BK$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CF$25:$CF$65,BK$25:BK$65)</f>
         <v>0</v>
       </c>
       <c r="BL85" s="589">
-        <f>+SUMPRODUCT(ProDegPaths!$CE$25:$CE$65,BL$25:BL$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CF$25:$CF$65,BL$25:BL$65)</f>
         <v>0</v>
       </c>
       <c r="BM85" s="301"/>
@@ -41344,26 +41344,26 @@
       <c r="G86" s="590"/>
       <c r="H86" s="595"/>
       <c r="L86" s="596">
-        <f t="shared" si="34"/>
+        <f t="shared" si="33"/>
         <v>15</v>
       </c>
       <c r="M86" s="597">
         <v>3</v>
       </c>
       <c r="N86" s="598">
-        <f t="shared" si="33"/>
+        <f t="shared" si="32"/>
         <v>0.2</v>
       </c>
       <c r="O86" s="599">
+        <f t="shared" si="34"/>
+        <v>14</v>
+      </c>
+      <c r="P86" s="599">
         <f t="shared" si="35"/>
-        <v>14</v>
-      </c>
-      <c r="P86" s="599">
-        <f t="shared" si="36"/>
         <v>12</v>
       </c>
       <c r="Q86" s="600">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>10</v>
       </c>
       <c r="S86" s="624" t="s">
@@ -41497,39 +41497,39 @@
       <c r="BA86" s="415"/>
       <c r="BB86" s="295"/>
       <c r="BD86" s="587">
-        <f>+SUMPRODUCT(ProDegPaths!$CF$25:$CF$65,BD$25:BD$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CG$25:$CG$65,BD$25:BD$65)+SUMPRODUCT(ProDegPaths!$CH$25:$CH$65,BD$25:BD$65)</f>
         <v>0</v>
       </c>
       <c r="BE86" s="588">
-        <f>+SUMPRODUCT(ProDegPaths!$CF$25:$CF$65,BE$25:BE$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CG$25:$CG$65,BE$25:BE$65)+SUMPRODUCT(ProDegPaths!$CH$25:$CH$65,BE$25:BE$65)</f>
         <v>0</v>
       </c>
       <c r="BF86" s="588">
-        <f>+SUMPRODUCT(ProDegPaths!$CF$25:$CF$65,BF$25:BF$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CG$25:$CG$65,BF$25:BF$65)+SUMPRODUCT(ProDegPaths!$CH$25:$CH$65,BF$25:BF$65)</f>
         <v>0</v>
       </c>
       <c r="BG86" s="588">
-        <f>+SUMPRODUCT(ProDegPaths!$CF$25:$CF$65,BG$25:BG$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CG$25:$CG$65,BG$25:BG$65)+SUMPRODUCT(ProDegPaths!$CH$25:$CH$65,BG$25:BG$65)</f>
         <v>0</v>
       </c>
       <c r="BH86" s="588">
-        <f>+SUMPRODUCT(ProDegPaths!$CF$25:$CF$65,BH$25:BH$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CG$25:$CG$65,BH$25:BH$65)+SUMPRODUCT(ProDegPaths!$CH$25:$CH$65,BH$25:BH$65)</f>
         <v>0</v>
       </c>
       <c r="BI86" s="589">
-        <f>+SUMPRODUCT(ProDegPaths!$CF$25:$CF$65,BI$25:BI$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CG$25:$CG$65,BI$25:BI$65)+SUMPRODUCT(ProDegPaths!$CH$25:$CH$65,BI$25:BI$65)</f>
         <v>0</v>
       </c>
       <c r="BJ86" s="589">
-        <f>+SUMPRODUCT(ProDegPaths!$CF$25:$CF$65,BJ$25:BJ$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CG$25:$CG$65,BJ$25:BJ$65)+SUMPRODUCT(ProDegPaths!$CH$25:$CH$65,BJ$25:BJ$65)</f>
         <v>0</v>
       </c>
       <c r="BK86" s="589">
-        <f>+SUMPRODUCT(ProDegPaths!$CF$25:$CF$65,BK$25:BK$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CG$25:$CG$65,BK$25:BK$65)+SUMPRODUCT(ProDegPaths!$CH$25:$CH$65,BK$25:BK$65)</f>
         <v>0</v>
       </c>
       <c r="BL86" s="589">
-        <f>+SUMPRODUCT(ProDegPaths!$CF$25:$CF$65,BL$25:BL$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CG$25:$CG$65,BL$25:BL$65)+SUMPRODUCT(ProDegPaths!$CH$25:$CH$65,BL$25:BL$65)</f>
         <v>0</v>
       </c>
       <c r="BM86" s="301"/>
@@ -41674,39 +41674,39 @@
       <c r="BA87" s="415"/>
       <c r="BB87" s="295"/>
       <c r="BD87" s="587">
-        <f>+SUMPRODUCT(ProDegPaths!$CG$25:$CG$65,BD$25:BD$65)+SUMPRODUCT(ProDegPaths!$CH$25:$CH$65,BD$25:BD$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CI$25:$CI$65,BD$25:BD$65)</f>
         <v>0</v>
       </c>
       <c r="BE87" s="588">
-        <f>+SUMPRODUCT(ProDegPaths!$CG$25:$CG$65,BE$25:BE$65)+SUMPRODUCT(ProDegPaths!$CH$25:$CH$65,BE$25:BE$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CI$25:$CI$65,BE$25:BE$65)</f>
         <v>0</v>
       </c>
       <c r="BF87" s="588">
-        <f>+SUMPRODUCT(ProDegPaths!$CG$25:$CG$65,BF$25:BF$65)+SUMPRODUCT(ProDegPaths!$CH$25:$CH$65,BF$25:BF$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CI$25:$CI$65,BF$25:BF$65)</f>
         <v>0</v>
       </c>
       <c r="BG87" s="588">
-        <f>+SUMPRODUCT(ProDegPaths!$CG$25:$CG$65,BG$25:BG$65)+SUMPRODUCT(ProDegPaths!$CH$25:$CH$65,BG$25:BG$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CI$25:$CI$65,BG$25:BG$65)</f>
         <v>0</v>
       </c>
       <c r="BH87" s="588">
-        <f>+SUMPRODUCT(ProDegPaths!$CG$25:$CG$65,BH$25:BH$65)+SUMPRODUCT(ProDegPaths!$CH$25:$CH$65,BH$25:BH$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CI$25:$CI$65,BH$25:BH$65)</f>
         <v>0</v>
       </c>
       <c r="BI87" s="589">
-        <f>+SUMPRODUCT(ProDegPaths!$CG$25:$CG$65,BI$25:BI$65)+SUMPRODUCT(ProDegPaths!$CH$25:$CH$65,BI$25:BI$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CI$25:$CI$65,BI$25:BI$65)</f>
         <v>0</v>
       </c>
       <c r="BJ87" s="589">
-        <f>+SUMPRODUCT(ProDegPaths!$CG$25:$CG$65,BJ$25:BJ$65)+SUMPRODUCT(ProDegPaths!$CH$25:$CH$65,BJ$25:BJ$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CI$25:$CI$65,BJ$25:BJ$65)</f>
         <v>0</v>
       </c>
       <c r="BK87" s="589">
-        <f>+SUMPRODUCT(ProDegPaths!$CG$25:$CG$65,BK$25:BK$65)+SUMPRODUCT(ProDegPaths!$CH$25:$CH$65,BK$25:BK$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CI$25:$CI$65,BK$25:BK$65)</f>
         <v>0</v>
       </c>
       <c r="BL87" s="589">
-        <f>+SUMPRODUCT(ProDegPaths!$CG$25:$CG$65,BL$25:BL$65)+SUMPRODUCT(ProDegPaths!$CH$25:$CH$65,BL$25:BL$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CI$25:$CI$65,BL$25:BL$65)</f>
         <v>0</v>
       </c>
       <c r="BM87" s="301"/>
@@ -41855,39 +41855,39 @@
       <c r="BA88" s="415"/>
       <c r="BB88" s="295"/>
       <c r="BD88" s="587">
-        <f>+SUMPRODUCT(ProDegPaths!$CI$25:$CI$65,BD$25:BD$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CJ$25:$CJ$65,BD$25:BD$65)</f>
         <v>0</v>
       </c>
       <c r="BE88" s="588">
-        <f>+SUMPRODUCT(ProDegPaths!$CI$25:$CI$65,BE$25:BE$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CJ$25:$CJ$65,BE$25:BE$65)</f>
         <v>0</v>
       </c>
       <c r="BF88" s="588">
-        <f>+SUMPRODUCT(ProDegPaths!$CI$25:$CI$65,BF$25:BF$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CJ$25:$CJ$65,BF$25:BF$65)</f>
         <v>0</v>
       </c>
       <c r="BG88" s="588">
-        <f>+SUMPRODUCT(ProDegPaths!$CI$25:$CI$65,BG$25:BG$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CJ$25:$CJ$65,BG$25:BG$65)</f>
         <v>0</v>
       </c>
       <c r="BH88" s="588">
-        <f>+SUMPRODUCT(ProDegPaths!$CI$25:$CI$65,BH$25:BH$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CJ$25:$CJ$65,BH$25:BH$65)</f>
         <v>0</v>
       </c>
       <c r="BI88" s="589">
-        <f>+SUMPRODUCT(ProDegPaths!$CI$25:$CI$65,BI$25:BI$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CJ$25:$CJ$65,BI$25:BI$65)</f>
         <v>0</v>
       </c>
       <c r="BJ88" s="589">
-        <f>+SUMPRODUCT(ProDegPaths!$CI$25:$CI$65,BJ$25:BJ$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CJ$25:$CJ$65,BJ$25:BJ$65)</f>
         <v>0</v>
       </c>
       <c r="BK88" s="589">
-        <f>+SUMPRODUCT(ProDegPaths!$CI$25:$CI$65,BK$25:BK$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CJ$25:$CJ$65,BK$25:BK$65)</f>
         <v>0</v>
       </c>
       <c r="BL88" s="589">
-        <f>+SUMPRODUCT(ProDegPaths!$CI$25:$CI$65,BL$25:BL$65)</f>
+        <f>+SUMPRODUCT(ProDegPaths!$CJ$25:$CJ$65,BL$25:BL$65)</f>
         <v>0</v>
       </c>
       <c r="BM88" s="301"/>
@@ -41914,211 +41914,175 @@
       </c>
       <c r="T89" s="647"/>
       <c r="V89" s="604">
-        <f t="shared" ref="V89:AZ89" si="37">+SUMPRODUCT($F$25:$F$65,V$25:V$65)</f>
+        <f t="shared" ref="V89:AZ89" si="36">+SUMPRODUCT($F$25:$F$65,V$25:V$65)</f>
         <v>0</v>
       </c>
       <c r="W89" s="605">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="X89" s="605">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="Y89" s="605">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="Z89" s="605">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="AA89" s="605">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="AB89" s="605">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="AC89" s="605">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="AD89" s="605">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="AE89" s="605">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="AF89" s="605">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="AG89" s="605">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="AH89" s="605">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="AI89" s="605">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="AJ89" s="605">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="AK89" s="605">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="AL89" s="605">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="AM89" s="605">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="AN89" s="605">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="AO89" s="605">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="AP89" s="605">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="AQ89" s="605">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="AR89" s="605">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="AS89" s="605">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="AT89" s="605">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="AU89" s="605">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="AV89" s="605">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="AW89" s="605">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="AX89" s="605">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="AY89" s="605">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="AZ89" s="606">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="BA89" s="415"/>
       <c r="BB89" s="295"/>
-      <c r="BD89" s="587">
-        <f>+SUMPRODUCT(ProDegPaths!$CJ$25:$CJ$65,BD$25:BD$65)</f>
-        <v>0</v>
-      </c>
-      <c r="BE89" s="588">
-        <f>+SUMPRODUCT(ProDegPaths!$CJ$25:$CJ$65,BE$25:BE$65)</f>
-        <v>0</v>
-      </c>
-      <c r="BF89" s="588">
-        <f>+SUMPRODUCT(ProDegPaths!$CJ$25:$CJ$65,BF$25:BF$65)</f>
-        <v>0</v>
-      </c>
-      <c r="BG89" s="588">
-        <f>+SUMPRODUCT(ProDegPaths!$CJ$25:$CJ$65,BG$25:BG$65)</f>
-        <v>0</v>
-      </c>
-      <c r="BH89" s="588">
-        <f>+SUMPRODUCT(ProDegPaths!$CJ$25:$CJ$65,BH$25:BH$65)</f>
-        <v>0</v>
-      </c>
-      <c r="BI89" s="589">
-        <f>+SUMPRODUCT(ProDegPaths!$CJ$25:$CJ$65,BI$25:BI$65)</f>
-        <v>0</v>
-      </c>
-      <c r="BJ89" s="589">
-        <f>+SUMPRODUCT(ProDegPaths!$CJ$25:$CJ$65,BJ$25:BJ$65)</f>
-        <v>0</v>
-      </c>
-      <c r="BK89" s="589">
-        <f>+SUMPRODUCT(ProDegPaths!$CJ$25:$CJ$65,BK$25:BK$65)</f>
-        <v>0</v>
-      </c>
-      <c r="BL89" s="589">
-        <f>+SUMPRODUCT(ProDegPaths!$CJ$25:$CJ$65,BL$25:BL$65)</f>
+      <c r="BD89" s="604">
+        <f t="shared" ref="BD89:BL89" si="37">+SUMPRODUCT($F$25:$F$65,BD$25:BD$65)</f>
+        <v>0</v>
+      </c>
+      <c r="BE89" s="605">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="BF89" s="605">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="BG89" s="605">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="BH89" s="605">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="BI89" s="606">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="BJ89" s="606">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="BK89" s="606">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="BL89" s="606">
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="BM89" s="301"/>
       <c r="BN89" s="295"/>
     </row>
-    <row r="90" spans="4:66" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="4:66" ht="14.4" thickTop="1" x14ac:dyDescent="0.3">
       <c r="Q90" s="538"/>
       <c r="T90" s="647"/>
       <c r="BA90" s="415"/>
       <c r="BB90" s="295"/>
-      <c r="BD90" s="604">
-        <f t="shared" ref="BD90:BL90" si="38">+SUMPRODUCT($F$25:$F$65,BD$25:BD$65)</f>
-        <v>0</v>
-      </c>
-      <c r="BE90" s="605">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="BF90" s="605">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="BG90" s="605">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="BH90" s="605">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="BI90" s="606">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="BJ90" s="606">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="BK90" s="606">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="BL90" s="606">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
       <c r="BM90" s="301"/>
       <c r="BN90" s="295"/>
     </row>
@@ -42983,7 +42947,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BD78:BF90 BK78:BK90 BH78:BH90 BM78:BM90">
+  <conditionalFormatting sqref="BD77:BF89 BK77:BK89 BH77:BH89 BM78:BM90">
     <cfRule type="cellIs" dxfId="443" priority="549" stopIfTrue="1" operator="notBetween">
       <formula>-0.000001</formula>
       <formula>0.000001</formula>
@@ -43182,7 +43146,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BI78:BI90">
+  <conditionalFormatting sqref="BI77:BI89">
     <cfRule type="cellIs" dxfId="399" priority="500" stopIfTrue="1" operator="notBetween">
       <formula>-0.000001</formula>
       <formula>0.000001</formula>
@@ -43231,7 +43195,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BG78:BG90">
+  <conditionalFormatting sqref="BG77:BG89">
     <cfRule type="cellIs" dxfId="388" priority="489" stopIfTrue="1" operator="notBetween">
       <formula>-0.000001</formula>
       <formula>0.000001</formula>
@@ -44001,7 +43965,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BJ78:BJ90">
+  <conditionalFormatting sqref="BJ77:BJ89">
     <cfRule type="cellIs" dxfId="216" priority="255" stopIfTrue="1" operator="notBetween">
       <formula>-0.000001</formula>
       <formula>0.000001</formula>
@@ -44642,84 +44606,12 @@
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BD77:BE77 BH77">
-    <cfRule type="cellIs" dxfId="68" priority="74" stopIfTrue="1" operator="lessThanOrEqual">
-      <formula>-0.00001</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="75" stopIfTrue="1" operator="greaterThan">
-      <formula>0.00001</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="76" stopIfTrue="1" operator="between">
-      <formula>-0.00001</formula>
-      <formula>0.00001</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BK77">
-    <cfRule type="cellIs" dxfId="65" priority="71" stopIfTrue="1" operator="lessThanOrEqual">
-      <formula>-0.00001</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="72" stopIfTrue="1" operator="greaterThan">
-      <formula>0.00001</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="73" stopIfTrue="1" operator="between">
-      <formula>-0.00001</formula>
-      <formula>0.00001</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BF77">
-    <cfRule type="cellIs" dxfId="62" priority="68" stopIfTrue="1" operator="lessThanOrEqual">
-      <formula>-0.00001</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="69" stopIfTrue="1" operator="greaterThan">
-      <formula>0.00001</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="70" stopIfTrue="1" operator="between">
-      <formula>-0.00001</formula>
-      <formula>0.00001</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BI77">
-    <cfRule type="cellIs" dxfId="59" priority="65" stopIfTrue="1" operator="lessThanOrEqual">
-      <formula>-0.00001</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="66" stopIfTrue="1" operator="greaterThan">
-      <formula>0.00001</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="67" stopIfTrue="1" operator="between">
-      <formula>-0.00001</formula>
-      <formula>0.00001</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BG77">
-    <cfRule type="cellIs" dxfId="56" priority="62" stopIfTrue="1" operator="lessThanOrEqual">
-      <formula>-0.00001</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="63" stopIfTrue="1" operator="greaterThan">
-      <formula>0.00001</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="64" stopIfTrue="1" operator="between">
-      <formula>-0.00001</formula>
-      <formula>0.00001</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BJ77">
-    <cfRule type="cellIs" dxfId="53" priority="32" stopIfTrue="1" operator="lessThanOrEqual">
-      <formula>-0.00001</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="33" stopIfTrue="1" operator="greaterThan">
-      <formula>0.00001</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="34" stopIfTrue="1" operator="between">
-      <formula>-0.00001</formula>
-      <formula>0.00001</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="BL66 BL25:BL58 BL61:BL64">
     <cfRule type="cellIs" dxfId="50" priority="22" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BL78:BL90">
+  <conditionalFormatting sqref="BL77:BL89">
     <cfRule type="cellIs" dxfId="49" priority="20" stopIfTrue="1" operator="notBetween">
       <formula>-0.000001</formula>
       <formula>0.000001</formula>
@@ -44778,18 +44670,6 @@
   <conditionalFormatting sqref="BL59">
     <cfRule type="cellIs" dxfId="36" priority="8" stopIfTrue="1" operator="equal">
       <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BL77">
-    <cfRule type="cellIs" dxfId="35" priority="5" stopIfTrue="1" operator="lessThanOrEqual">
-      <formula>-0.00001</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="6" stopIfTrue="1" operator="greaterThan">
-      <formula>0.00001</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="7" stopIfTrue="1" operator="between">
-      <formula>-0.00001</formula>
-      <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M55">

</xml_diff>

<commit_message>
Generalised swap with NADH, changed collection of PrintResults and colormap generation
</commit_message>
<xml_diff>
--- a/PropionateOxidation.xlsx
+++ b/PropionateOxidation.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" updateLinks="always"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB40F651-4247-4FEA-BE0F-AEDEAB30D0AA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA58DFA-0460-4AE3-A1C1-4DF4D39C2143}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{B1DDE01B-6290-4C58-94E8-4710908F5800}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B1DDE01B-6290-4C58-94E8-4710908F5800}"/>
   </bookViews>
   <sheets>
     <sheet name="ProDegPaths" sheetId="12" r:id="rId1"/>
@@ -124,7 +124,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Author:</t>
         </r>
@@ -133,7 +133,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 eD must be identified here</t>
@@ -13781,7 +13781,7 @@
     <numFmt numFmtId="170" formatCode="0.0000000000000"/>
     <numFmt numFmtId="171" formatCode="#/3"/>
   </numFmts>
-  <fonts count="78" x14ac:knownFonts="1">
+  <fonts count="76" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -14305,19 +14305,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="22">
@@ -17354,7 +17341,7 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Normal 2 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
-  <dxfs count="525">
+  <dxfs count="504">
     <dxf>
       <font>
         <color theme="2" tint="-9.9948118533890809E-2"/>
@@ -17669,38 +17656,6 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="47"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="17"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <condense val="0"/>
         <extend val="0"/>
         <color indexed="29"/>
@@ -17842,198 +17797,6 @@
         <condense val="0"/>
         <extend val="0"/>
         <color indexed="29"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="47"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="17"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="47"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="17"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="47"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="17"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="47"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="17"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="47"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="17"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="47"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="17"/>
       </font>
     </dxf>
     <dxf>
@@ -23092,7 +22855,7 @@
   </sheetPr>
   <dimension ref="A1:CU144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE11" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="AE11" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AR33" sqref="AR33"/>
     </sheetView>
   </sheetViews>
@@ -42569,2106 +42332,2106 @@
     <mergeCell ref="D117:G117"/>
   </mergeCells>
   <conditionalFormatting sqref="L65:O65 L25:L27 N26:N27 BB25:BB27 Q65 R45:R54 R25:R27 O45:O54 L66:Q66 BM66:BN66 L45:L56 N30:N34 M30:M31 BM29:BM31 R62 L62 N62:P62 BM59:BM65 Q61:Q63 L58 BN49:BN65 N58:R58 L59:R59 BN44:BN45 O44:P44 R29:R34 O25:P34 Q27:Q34 BN29:BN34 BB29:BB34 BC25:BC34 O43:R43 L29:L36 L37:R42 BM35:BN43 BB35:BC66 M35:R36 L43:M43 V66:AK67 U25:U65 AM66:AZ67">
-    <cfRule type="cellIs" dxfId="524" priority="631" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="503" priority="631" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CP60:CU61 AK60 Q60:S60 L60:O60 Y60:AC60 AY60 AE60:AF60 AH60:AI60 AM60 AO60:AS60">
-    <cfRule type="cellIs" dxfId="523" priority="632" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="502" priority="632" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BA69 BA71:BA72 BA76 AW71:AW72 AW76 Y76:AC76 Y71:AC72 AM76:AR76 AM71:AR72 AE71:AF72 AE76:AF76 AH76 AH71:AH72 BM77 BE67:BG67 BI67:BJ68 BF68:BG68 BD69:BG69 BI69:BK69">
-    <cfRule type="cellIs" dxfId="522" priority="626" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="501" priority="626" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="521" priority="627" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="500" priority="627" stopIfTrue="1" operator="greaterThan">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="520" priority="628" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="499" priority="628" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y77:AC89 AW77:AW89 AK77:AK89 AE77:AF89 AH77:AI89 AM77:AS89 BA78:BA90 AZ77:AZ89">
-    <cfRule type="cellIs" dxfId="519" priority="629" stopIfTrue="1" operator="notBetween">
+    <cfRule type="cellIs" dxfId="498" priority="629" stopIfTrue="1" operator="notBetween">
       <formula>-0.000001</formula>
       <formula>0.000001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="518" priority="630" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="497" priority="630" stopIfTrue="1" operator="between">
       <formula>-0.000001</formula>
       <formula>0.000001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y25:Y27 AM65 BK66 Y65:AC65 AX65 AE65:AF65 AH65:AI65 AS59 AS55:AX58 BD66:BI66 AY61:AY65 AO61:AR61 V61:AK64 AW61:AX64 BD61:BI64 V58:Z59 AM55:AN59 AY49:AY59 AA55:AI59 AJ58:AK59 AO44:AR59 Z44 AY45:AY46 AK44 AA25:AI34 V29:Z34 AJ29:AK34 V35:AK43 BG25:BI58 BD29:BF54 AM44:AN44 AM61:AN64 AS44:AV54 BK25:BK58 BK61:BK64 AO62:AV65 AM25:AY43">
-    <cfRule type="cellIs" dxfId="517" priority="633" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="496" priority="633" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BA73:BA75 AW73:AW75 Y73:AC75 AM73:AR75 AE73:AF75 AH73:AH75">
-    <cfRule type="cellIs" dxfId="516" priority="634" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="495" priority="634" stopIfTrue="1" operator="greaterThan">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="515" priority="635" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="494" priority="635" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="514" priority="636" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="493" priority="636" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CP65:CU65 CP25:CU59">
-    <cfRule type="cellIs" dxfId="513" priority="624" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="492" priority="624" stopIfTrue="1" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="512" priority="625" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="491" priority="625" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB28 L28 N28 R28">
-    <cfRule type="cellIs" dxfId="511" priority="622" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="490" priority="622" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y28">
-    <cfRule type="cellIs" dxfId="510" priority="623" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="489" priority="623" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y55">
-    <cfRule type="cellIs" dxfId="509" priority="621" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="488" priority="621" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L55 O55 R55">
-    <cfRule type="cellIs" dxfId="508" priority="620" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="487" priority="620" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK56:AK57">
-    <cfRule type="cellIs" dxfId="507" priority="602" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="486" priority="602" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI71:AI72 AI76 AS76 AS71:AS72">
-    <cfRule type="cellIs" dxfId="506" priority="614" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="485" priority="614" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="505" priority="615" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="484" priority="615" stopIfTrue="1" operator="greaterThan">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="504" priority="616" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="483" priority="616" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI73:AI75 AS73:AS75">
-    <cfRule type="cellIs" dxfId="503" priority="617" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="482" priority="617" stopIfTrue="1" operator="greaterThan">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="502" priority="618" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="481" priority="618" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="501" priority="619" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="480" priority="619" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y56:Y57">
-    <cfRule type="cellIs" dxfId="500" priority="613" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="479" priority="613" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L56 N56:O56 Q56:R56">
-    <cfRule type="cellIs" dxfId="499" priority="612" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="478" priority="612" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK76 AK71:AK72">
-    <cfRule type="cellIs" dxfId="498" priority="605" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="477" priority="605" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="497" priority="606" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="476" priority="606" stopIfTrue="1" operator="greaterThan">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="496" priority="607" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="475" priority="607" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK25:AK27 AK65">
-    <cfRule type="cellIs" dxfId="495" priority="608" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="474" priority="608" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK73:AK75">
-    <cfRule type="cellIs" dxfId="494" priority="609" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="473" priority="609" stopIfTrue="1" operator="greaterThan">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="493" priority="610" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="472" priority="610" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="492" priority="611" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="471" priority="611" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK28">
-    <cfRule type="cellIs" dxfId="491" priority="604" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="470" priority="604" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK55">
-    <cfRule type="cellIs" dxfId="490" priority="603" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="469" priority="603" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB113:BB127">
-    <cfRule type="cellIs" dxfId="489" priority="601" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="468" priority="601" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB98:BB112">
-    <cfRule type="cellIs" dxfId="488" priority="600" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="467" priority="600" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB94:BB96">
-    <cfRule type="cellIs" dxfId="487" priority="599" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="466" priority="599" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB97">
-    <cfRule type="cellIs" dxfId="486" priority="598" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="465" priority="598" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AZ71:AZ72 AZ76">
-    <cfRule type="cellIs" dxfId="485" priority="592" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="464" priority="592" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="484" priority="593" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="463" priority="593" stopIfTrue="1" operator="greaterThan">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="483" priority="594" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="462" priority="594" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AZ73:AZ75">
-    <cfRule type="cellIs" dxfId="482" priority="595" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="461" priority="595" stopIfTrue="1" operator="greaterThan">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="481" priority="596" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="460" priority="596" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="480" priority="597" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="459" priority="597" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R44">
-    <cfRule type="cellIs" dxfId="479" priority="591" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="458" priority="591" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z25:Z27">
-    <cfRule type="cellIs" dxfId="478" priority="590" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="457" priority="590" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z28">
-    <cfRule type="cellIs" dxfId="477" priority="589" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="456" priority="589" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z55">
-    <cfRule type="cellIs" dxfId="476" priority="588" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="455" priority="588" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z56:Z57">
-    <cfRule type="cellIs" dxfId="475" priority="587" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="454" priority="587" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H68">
-    <cfRule type="cellIs" dxfId="474" priority="586" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="453" priority="586" operator="greaterThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M25">
-    <cfRule type="cellIs" dxfId="473" priority="585" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="452" priority="585" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M29">
-    <cfRule type="cellIs" dxfId="472" priority="584" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="451" priority="584" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q25">
-    <cfRule type="cellIs" dxfId="471" priority="583" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="450" priority="583" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q26:Q28">
-    <cfRule type="cellIs" dxfId="470" priority="582" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="449" priority="582" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N25:N44">
-    <cfRule type="cellIs" dxfId="469" priority="581" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="448" priority="581" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N43">
-    <cfRule type="cellIs" dxfId="468" priority="580" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="447" priority="580" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N29">
-    <cfRule type="cellIs" dxfId="467" priority="579" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="446" priority="579" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q43">
-    <cfRule type="cellIs" dxfId="466" priority="578" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="445" priority="578" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q32:Q34">
-    <cfRule type="cellIs" dxfId="465" priority="577" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="444" priority="577" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N44">
-    <cfRule type="cellIs" dxfId="464" priority="575" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="443" priority="575" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M25:M30">
-    <cfRule type="cellIs" dxfId="463" priority="569" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="442" priority="569" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M56 M44:M54">
-    <cfRule type="cellIs" dxfId="462" priority="568" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="441" priority="568" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N32:N34">
-    <cfRule type="cellIs" dxfId="461" priority="567" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="440" priority="567" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M32:M34">
-    <cfRule type="cellIs" dxfId="460" priority="566" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="439" priority="566" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q26">
-    <cfRule type="cellIs" dxfId="459" priority="562" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="438" priority="562" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N55">
-    <cfRule type="cellIs" dxfId="458" priority="564" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="437" priority="564" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q55">
-    <cfRule type="cellIs" dxfId="457" priority="563" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="436" priority="563" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P65 P45:P54">
-    <cfRule type="cellIs" dxfId="456" priority="560" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="435" priority="560" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P60">
-    <cfRule type="cellIs" dxfId="455" priority="561" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="434" priority="561" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P55">
-    <cfRule type="cellIs" dxfId="454" priority="559" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="433" priority="559" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P56">
-    <cfRule type="cellIs" dxfId="453" priority="558" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="432" priority="558" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q45:Q54">
-    <cfRule type="cellIs" dxfId="452" priority="557" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="431" priority="557" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q44">
-    <cfRule type="cellIs" dxfId="451" priority="556" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="430" priority="556" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q44">
-    <cfRule type="cellIs" dxfId="450" priority="555" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="429" priority="555" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y44:Y54 AA44:AC54 AX44 AE44:AF54 AH44:AI54 AX47:AX54">
-    <cfRule type="cellIs" dxfId="449" priority="552" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="428" priority="552" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK45:AK54 AM45:AM54">
-    <cfRule type="cellIs" dxfId="448" priority="554" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="427" priority="554" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z45:Z54">
-    <cfRule type="cellIs" dxfId="447" priority="553" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="426" priority="553" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BN98:BN112">
-    <cfRule type="cellIs" dxfId="446" priority="522" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="425" priority="522" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS61 AU61:AV61">
-    <cfRule type="cellIs" dxfId="445" priority="551" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="424" priority="551" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BD25:BD27 BD65 BD58">
-    <cfRule type="cellIs" dxfId="444" priority="528" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="423" priority="528" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BD77:BF89 BK77:BK89 BH77:BH89 BM78:BM90">
-    <cfRule type="cellIs" dxfId="443" priority="549" stopIfTrue="1" operator="notBetween">
+    <cfRule type="cellIs" dxfId="422" priority="549" stopIfTrue="1" operator="notBetween">
       <formula>-0.000001</formula>
       <formula>0.000001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="442" priority="550" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="421" priority="550" stopIfTrue="1" operator="between">
       <formula>-0.000001</formula>
       <formula>0.000001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BC113:BC127">
-    <cfRule type="cellIs" dxfId="441" priority="548" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="420" priority="548" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BC98:BC112">
-    <cfRule type="cellIs" dxfId="440" priority="547" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="419" priority="547" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BC94:BC96">
-    <cfRule type="cellIs" dxfId="439" priority="546" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="418" priority="546" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BC97">
-    <cfRule type="cellIs" dxfId="438" priority="545" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="417" priority="545" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BM49:BM51 BM46:BN46 BM44">
-    <cfRule type="cellIs" dxfId="437" priority="539" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="416" priority="539" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BE60:BF60 BH60">
-    <cfRule type="cellIs" dxfId="436" priority="540" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="415" priority="540" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BD76:BE76 BD71:BE72 BH71:BH72 BH76">
-    <cfRule type="cellIs" dxfId="435" priority="536" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="414" priority="536" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="434" priority="537" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="413" priority="537" stopIfTrue="1" operator="greaterThan">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="433" priority="538" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="412" priority="538" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BE25:BF28 BE55:BF58 BE65:BF65 BH65">
-    <cfRule type="cellIs" dxfId="432" priority="541" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="411" priority="541" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BD73:BE75 BH73:BH75">
-    <cfRule type="cellIs" dxfId="431" priority="542" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="410" priority="542" stopIfTrue="1" operator="greaterThan">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="430" priority="543" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="409" priority="543" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="429" priority="544" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="408" priority="544" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BN47:BN48">
-    <cfRule type="cellIs" dxfId="428" priority="535" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="407" priority="535" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BD56:BD57">
-    <cfRule type="cellIs" dxfId="427" priority="524" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="406" priority="524" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BM48 BM25:BN27">
-    <cfRule type="cellIs" dxfId="426" priority="533" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="405" priority="533" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BD60">
-    <cfRule type="cellIs" dxfId="425" priority="534" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="404" priority="534" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BM71:BM76">
-    <cfRule type="cellIs" dxfId="424" priority="530" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="403" priority="530" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="423" priority="531" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="402" priority="531" stopIfTrue="1" operator="greaterThan">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="422" priority="532" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="401" priority="532" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BM28:BN28">
-    <cfRule type="cellIs" dxfId="421" priority="529" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="400" priority="529" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BD28">
-    <cfRule type="cellIs" dxfId="420" priority="526" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="399" priority="526" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BD55">
-    <cfRule type="cellIs" dxfId="419" priority="525" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="398" priority="525" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BD60">
-    <cfRule type="cellIs" dxfId="418" priority="527" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="397" priority="527" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BN113:BN127">
-    <cfRule type="cellIs" dxfId="417" priority="523" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="396" priority="523" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BN94:BN96">
-    <cfRule type="cellIs" dxfId="416" priority="521" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="395" priority="521" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BN97">
-    <cfRule type="cellIs" dxfId="415" priority="520" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="394" priority="520" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BK71:BK72 BK76">
-    <cfRule type="cellIs" dxfId="414" priority="514" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="393" priority="514" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="413" priority="515" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="392" priority="515" stopIfTrue="1" operator="greaterThan">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="412" priority="516" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="391" priority="516" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BK73:BK75">
-    <cfRule type="cellIs" dxfId="411" priority="517" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="390" priority="517" stopIfTrue="1" operator="greaterThan">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="410" priority="518" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="389" priority="518" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="409" priority="519" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="388" priority="519" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BK60">
-    <cfRule type="cellIs" dxfId="408" priority="512" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="387" priority="512" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BK65">
-    <cfRule type="cellIs" dxfId="407" priority="513" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="386" priority="513" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BF76 BF71:BF72">
-    <cfRule type="cellIs" dxfId="406" priority="503" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="385" priority="503" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="405" priority="504" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="384" priority="504" stopIfTrue="1" operator="greaterThan">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="404" priority="505" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="383" priority="505" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BF73:BF75">
-    <cfRule type="cellIs" dxfId="403" priority="506" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="382" priority="506" stopIfTrue="1" operator="greaterThan">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="402" priority="507" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="381" priority="507" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="401" priority="508" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="380" priority="508" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BE59:BF59 BK59 BH59">
-    <cfRule type="cellIs" dxfId="400" priority="502" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="379" priority="502" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BI77:BI89">
-    <cfRule type="cellIs" dxfId="399" priority="500" stopIfTrue="1" operator="notBetween">
+    <cfRule type="cellIs" dxfId="378" priority="500" stopIfTrue="1" operator="notBetween">
       <formula>-0.000001</formula>
       <formula>0.000001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="398" priority="501" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="377" priority="501" stopIfTrue="1" operator="between">
       <formula>-0.000001</formula>
       <formula>0.000001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BI71:BI72 BI76">
-    <cfRule type="cellIs" dxfId="397" priority="494" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="376" priority="494" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="396" priority="495" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="375" priority="495" stopIfTrue="1" operator="greaterThan">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="395" priority="496" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="374" priority="496" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BI73:BI75">
-    <cfRule type="cellIs" dxfId="394" priority="497" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="373" priority="497" stopIfTrue="1" operator="greaterThan">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="393" priority="498" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="372" priority="498" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="392" priority="499" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="371" priority="499" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BI60">
-    <cfRule type="cellIs" dxfId="391" priority="492" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="370" priority="492" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BI65">
-    <cfRule type="cellIs" dxfId="390" priority="493" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="369" priority="493" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BI59">
-    <cfRule type="cellIs" dxfId="389" priority="491" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="368" priority="491" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BG77:BG89">
-    <cfRule type="cellIs" dxfId="388" priority="489" stopIfTrue="1" operator="notBetween">
+    <cfRule type="cellIs" dxfId="367" priority="489" stopIfTrue="1" operator="notBetween">
       <formula>-0.000001</formula>
       <formula>0.000001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="387" priority="490" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="366" priority="490" stopIfTrue="1" operator="between">
       <formula>-0.000001</formula>
       <formula>0.000001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BG60">
-    <cfRule type="cellIs" dxfId="386" priority="487" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="365" priority="487" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BG65">
-    <cfRule type="cellIs" dxfId="385" priority="488" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="364" priority="488" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BG76 BG71:BG72">
-    <cfRule type="cellIs" dxfId="384" priority="481" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="363" priority="481" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="383" priority="482" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="362" priority="482" stopIfTrue="1" operator="greaterThan">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="382" priority="483" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="361" priority="483" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BG73:BG75">
-    <cfRule type="cellIs" dxfId="381" priority="484" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="360" priority="484" stopIfTrue="1" operator="greaterThan">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="380" priority="485" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="359" priority="485" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="379" priority="486" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="358" priority="486" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BG59">
-    <cfRule type="cellIs" dxfId="378" priority="480" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="357" priority="480" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU77:AU89">
-    <cfRule type="cellIs" dxfId="377" priority="478" stopIfTrue="1" operator="notBetween">
+    <cfRule type="cellIs" dxfId="356" priority="478" stopIfTrue="1" operator="notBetween">
       <formula>-0.000001</formula>
       <formula>0.000001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="376" priority="479" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="355" priority="479" stopIfTrue="1" operator="between">
       <formula>-0.000001</formula>
       <formula>0.000001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU71:AU72 AU76">
-    <cfRule type="cellIs" dxfId="375" priority="472" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="354" priority="472" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="374" priority="473" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="353" priority="473" stopIfTrue="1" operator="greaterThan">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="373" priority="474" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="352" priority="474" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU73:AU75">
-    <cfRule type="cellIs" dxfId="372" priority="475" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="351" priority="475" stopIfTrue="1" operator="greaterThan">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="371" priority="476" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="350" priority="476" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="370" priority="477" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="349" priority="477" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AV77:AV89">
-    <cfRule type="cellIs" dxfId="369" priority="470" stopIfTrue="1" operator="notBetween">
+    <cfRule type="cellIs" dxfId="348" priority="470" stopIfTrue="1" operator="notBetween">
       <formula>-0.000001</formula>
       <formula>0.000001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="368" priority="471" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="347" priority="471" stopIfTrue="1" operator="between">
       <formula>-0.000001</formula>
       <formula>0.000001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AV71:AV72 AV76">
-    <cfRule type="cellIs" dxfId="367" priority="464" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="346" priority="464" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="366" priority="465" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="345" priority="465" stopIfTrue="1" operator="greaterThan">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="365" priority="466" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="344" priority="466" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AV73:AV75">
-    <cfRule type="cellIs" dxfId="364" priority="467" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="343" priority="467" stopIfTrue="1" operator="greaterThan">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="363" priority="468" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="342" priority="468" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="362" priority="469" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="341" priority="469" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU60:AV60">
-    <cfRule type="cellIs" dxfId="361" priority="462" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="340" priority="462" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU59:AV59">
-    <cfRule type="cellIs" dxfId="360" priority="463" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="339" priority="463" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AW60">
-    <cfRule type="cellIs" dxfId="359" priority="460" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="338" priority="460" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AW65">
-    <cfRule type="cellIs" dxfId="358" priority="461" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="337" priority="461" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AW45:AW50">
-    <cfRule type="cellIs" dxfId="357" priority="459" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="336" priority="459" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AW44">
-    <cfRule type="cellIs" dxfId="356" priority="458" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="335" priority="458" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AN60">
-    <cfRule type="cellIs" dxfId="355" priority="456" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="334" priority="456" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AN65">
-    <cfRule type="cellIs" dxfId="354" priority="457" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="333" priority="457" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AN45:AN54">
-    <cfRule type="cellIs" dxfId="353" priority="455" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="332" priority="455" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AY77:AY89">
-    <cfRule type="cellIs" dxfId="352" priority="453" stopIfTrue="1" operator="notBetween">
+    <cfRule type="cellIs" dxfId="331" priority="453" stopIfTrue="1" operator="notBetween">
       <formula>-0.000001</formula>
       <formula>0.000001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="351" priority="454" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="330" priority="454" stopIfTrue="1" operator="between">
       <formula>-0.000001</formula>
       <formula>0.000001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AY71:AY72 AY76">
-    <cfRule type="cellIs" dxfId="350" priority="447" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="329" priority="447" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="349" priority="448" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="328" priority="448" stopIfTrue="1" operator="greaterThan">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="348" priority="449" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="327" priority="449" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AY73:AY75">
-    <cfRule type="cellIs" dxfId="347" priority="450" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="326" priority="450" stopIfTrue="1" operator="greaterThan">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="346" priority="451" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="325" priority="451" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="345" priority="452" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="324" priority="452" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA67:AC67 AB66:AC66 Y66:Z67 AK67 AE66:AF67 AH66:AI67 AM66:AS67">
-    <cfRule type="cellIs" dxfId="344" priority="445" operator="equal">
+    <cfRule type="cellIs" dxfId="323" priority="445" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="343" priority="446" operator="equal">
+    <cfRule type="cellIs" dxfId="322" priority="446" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L57">
-    <cfRule type="cellIs" dxfId="342" priority="444" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="321" priority="444" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L57 O57 R57">
-    <cfRule type="cellIs" dxfId="341" priority="443" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="320" priority="443" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P57">
-    <cfRule type="cellIs" dxfId="340" priority="442" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="319" priority="442" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N57">
-    <cfRule type="cellIs" dxfId="339" priority="438" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="318" priority="438" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q57">
-    <cfRule type="cellIs" dxfId="338" priority="440" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="317" priority="440" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BD59">
-    <cfRule type="cellIs" dxfId="337" priority="439" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="316" priority="439" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA66">
-    <cfRule type="cellIs" dxfId="336" priority="436" operator="equal">
+    <cfRule type="cellIs" dxfId="315" priority="436" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="335" priority="437" operator="equal">
+    <cfRule type="cellIs" dxfId="314" priority="437" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK66">
-    <cfRule type="cellIs" dxfId="334" priority="433" operator="equal">
+    <cfRule type="cellIs" dxfId="313" priority="433" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="333" priority="434" operator="equal">
+    <cfRule type="cellIs" dxfId="312" priority="434" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AX60">
-    <cfRule type="cellIs" dxfId="332" priority="371" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="311" priority="371" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AX59">
-    <cfRule type="cellIs" dxfId="331" priority="372" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="310" priority="372" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AX77:AX89">
-    <cfRule type="cellIs" dxfId="330" priority="369" stopIfTrue="1" operator="notBetween">
+    <cfRule type="cellIs" dxfId="309" priority="369" stopIfTrue="1" operator="notBetween">
       <formula>-0.000001</formula>
       <formula>0.000001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="329" priority="370" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="308" priority="370" stopIfTrue="1" operator="between">
       <formula>-0.000001</formula>
       <formula>0.000001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AX71:AX72 AX76">
-    <cfRule type="cellIs" dxfId="328" priority="363" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="307" priority="363" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="327" priority="364" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="306" priority="364" stopIfTrue="1" operator="greaterThan">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="326" priority="365" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="305" priority="365" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AX73:AX75">
-    <cfRule type="cellIs" dxfId="325" priority="366" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="304" priority="366" stopIfTrue="1" operator="greaterThan">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="324" priority="367" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="303" priority="367" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="323" priority="368" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="302" priority="368" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M58">
-    <cfRule type="cellIs" dxfId="322" priority="362" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="301" priority="362" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P63">
-    <cfRule type="cellIs" dxfId="321" priority="346" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="300" priority="346" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N61:P61">
-    <cfRule type="cellIs" dxfId="320" priority="343" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="299" priority="343" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CP62:CU62">
-    <cfRule type="cellIs" dxfId="319" priority="360" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="298" priority="360" stopIfTrue="1" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="318" priority="361" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="297" priority="361" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CP64:CU64">
-    <cfRule type="cellIs" dxfId="317" priority="358" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="296" priority="358" stopIfTrue="1" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="316" priority="359" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="295" priority="359" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CP63:CU63">
-    <cfRule type="cellIs" dxfId="315" priority="356" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="294" priority="356" stopIfTrue="1" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="314" priority="357" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="293" priority="357" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R64 L64">
-    <cfRule type="cellIs" dxfId="313" priority="355" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="292" priority="355" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M64">
-    <cfRule type="cellIs" dxfId="312" priority="354" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="291" priority="354" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O64">
-    <cfRule type="cellIs" dxfId="311" priority="353" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="290" priority="353" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N64">
-    <cfRule type="cellIs" dxfId="310" priority="352" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="289" priority="352" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q64">
-    <cfRule type="cellIs" dxfId="309" priority="351" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="288" priority="351" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P64">
-    <cfRule type="cellIs" dxfId="308" priority="350" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="287" priority="350" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L63:M63 R63">
-    <cfRule type="cellIs" dxfId="307" priority="349" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="286" priority="349" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O63">
-    <cfRule type="cellIs" dxfId="306" priority="348" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="285" priority="348" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N63">
-    <cfRule type="cellIs" dxfId="305" priority="347" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="284" priority="347" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R61 L61">
-    <cfRule type="cellIs" dxfId="304" priority="345" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="283" priority="345" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M61:M64">
-    <cfRule type="cellIs" dxfId="303" priority="344" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="282" priority="344" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AT77:AT89">
-    <cfRule type="cellIs" dxfId="302" priority="341" stopIfTrue="1" operator="notBetween">
+    <cfRule type="cellIs" dxfId="281" priority="341" stopIfTrue="1" operator="notBetween">
       <formula>-0.000001</formula>
       <formula>0.000001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="301" priority="342" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="280" priority="342" stopIfTrue="1" operator="between">
       <formula>-0.000001</formula>
       <formula>0.000001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AT71:AT72 AT76">
-    <cfRule type="cellIs" dxfId="300" priority="335" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="279" priority="335" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="299" priority="336" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="278" priority="336" stopIfTrue="1" operator="greaterThan">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="298" priority="337" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="277" priority="337" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AT73:AT75">
-    <cfRule type="cellIs" dxfId="297" priority="338" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="276" priority="338" stopIfTrue="1" operator="greaterThan">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="296" priority="339" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="275" priority="339" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="295" priority="340" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="274" priority="340" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W56:W57">
-    <cfRule type="cellIs" dxfId="294" priority="304" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="273" priority="304" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AT67">
-    <cfRule type="cellIs" dxfId="293" priority="299" operator="equal">
+    <cfRule type="cellIs" dxfId="272" priority="299" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="292" priority="300" operator="equal">
+    <cfRule type="cellIs" dxfId="271" priority="300" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AT66">
-    <cfRule type="cellIs" dxfId="291" priority="297" operator="equal">
+    <cfRule type="cellIs" dxfId="270" priority="297" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="290" priority="298" operator="equal">
+    <cfRule type="cellIs" dxfId="269" priority="298" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V60">
-    <cfRule type="cellIs" dxfId="289" priority="330" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="268" priority="330" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V76 V71:V72">
-    <cfRule type="cellIs" dxfId="288" priority="325" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="267" priority="325" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="287" priority="326" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="266" priority="326" stopIfTrue="1" operator="greaterThan">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="286" priority="327" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="265" priority="327" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V77:V89">
-    <cfRule type="cellIs" dxfId="285" priority="328" stopIfTrue="1" operator="notBetween">
+    <cfRule type="cellIs" dxfId="264" priority="328" stopIfTrue="1" operator="notBetween">
       <formula>-0.000001</formula>
       <formula>0.000001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="284" priority="329" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="263" priority="329" stopIfTrue="1" operator="between">
       <formula>-0.000001</formula>
       <formula>0.000001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V25:V27 V65">
-    <cfRule type="cellIs" dxfId="283" priority="331" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="262" priority="331" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V73:V75">
-    <cfRule type="cellIs" dxfId="282" priority="332" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="261" priority="332" stopIfTrue="1" operator="greaterThan">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="281" priority="333" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="260" priority="333" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="280" priority="334" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="259" priority="334" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V28">
-    <cfRule type="cellIs" dxfId="279" priority="324" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="258" priority="324" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V55">
-    <cfRule type="cellIs" dxfId="278" priority="323" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="257" priority="323" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V56:V57">
-    <cfRule type="cellIs" dxfId="277" priority="322" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="256" priority="322" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V44:V54">
-    <cfRule type="cellIs" dxfId="276" priority="321" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="255" priority="321" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V67">
-    <cfRule type="cellIs" dxfId="275" priority="319" operator="equal">
+    <cfRule type="cellIs" dxfId="254" priority="319" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="274" priority="320" operator="equal">
+    <cfRule type="cellIs" dxfId="253" priority="320" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V66">
-    <cfRule type="cellIs" dxfId="273" priority="317" operator="equal">
+    <cfRule type="cellIs" dxfId="252" priority="317" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="272" priority="318" operator="equal">
+    <cfRule type="cellIs" dxfId="251" priority="318" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W60">
-    <cfRule type="cellIs" dxfId="271" priority="312" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="250" priority="312" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W76 W71:W72">
-    <cfRule type="cellIs" dxfId="270" priority="307" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="249" priority="307" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="269" priority="308" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="248" priority="308" stopIfTrue="1" operator="greaterThan">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="268" priority="309" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="247" priority="309" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W77:W89">
-    <cfRule type="cellIs" dxfId="267" priority="310" stopIfTrue="1" operator="notBetween">
+    <cfRule type="cellIs" dxfId="246" priority="310" stopIfTrue="1" operator="notBetween">
       <formula>-0.000001</formula>
       <formula>0.000001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="266" priority="311" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="245" priority="311" stopIfTrue="1" operator="between">
       <formula>-0.000001</formula>
       <formula>0.000001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W25:W27 W65">
-    <cfRule type="cellIs" dxfId="265" priority="313" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="244" priority="313" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W73:W75">
-    <cfRule type="cellIs" dxfId="264" priority="314" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="243" priority="314" stopIfTrue="1" operator="greaterThan">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="263" priority="315" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="242" priority="315" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="262" priority="316" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="241" priority="316" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W28">
-    <cfRule type="cellIs" dxfId="261" priority="306" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="240" priority="306" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W55">
-    <cfRule type="cellIs" dxfId="260" priority="305" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="239" priority="305" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W44:W54">
-    <cfRule type="cellIs" dxfId="259" priority="303" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="238" priority="303" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W66:W67">
-    <cfRule type="cellIs" dxfId="258" priority="301" operator="equal">
+    <cfRule type="cellIs" dxfId="237" priority="301" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="257" priority="302" operator="equal">
+    <cfRule type="cellIs" dxfId="236" priority="302" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X60">
-    <cfRule type="cellIs" dxfId="256" priority="295" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="235" priority="295" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X77:X89">
-    <cfRule type="cellIs" dxfId="255" priority="293" stopIfTrue="1" operator="notBetween">
+    <cfRule type="cellIs" dxfId="234" priority="293" stopIfTrue="1" operator="notBetween">
       <formula>-0.000001</formula>
       <formula>0.000001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="254" priority="294" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="233" priority="294" stopIfTrue="1" operator="between">
       <formula>-0.000001</formula>
       <formula>0.000001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X65">
-    <cfRule type="cellIs" dxfId="253" priority="296" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="232" priority="296" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X25:X27">
-    <cfRule type="cellIs" dxfId="252" priority="289" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="231" priority="289" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X76 X71:X72">
-    <cfRule type="cellIs" dxfId="251" priority="286" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="230" priority="286" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="250" priority="287" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="229" priority="287" stopIfTrue="1" operator="greaterThan">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="249" priority="288" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="228" priority="288" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X73:X75">
-    <cfRule type="cellIs" dxfId="248" priority="290" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="227" priority="290" stopIfTrue="1" operator="greaterThan">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="247" priority="291" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="226" priority="291" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="246" priority="292" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="225" priority="292" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X28">
-    <cfRule type="cellIs" dxfId="245" priority="285" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="224" priority="285" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X55">
-    <cfRule type="cellIs" dxfId="244" priority="284" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="223" priority="284" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X56:X57">
-    <cfRule type="cellIs" dxfId="243" priority="283" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="222" priority="283" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X44:X54">
-    <cfRule type="cellIs" dxfId="242" priority="282" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="221" priority="282" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X67">
-    <cfRule type="cellIs" dxfId="241" priority="280" operator="equal">
+    <cfRule type="cellIs" dxfId="220" priority="280" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="240" priority="281" operator="equal">
+    <cfRule type="cellIs" dxfId="219" priority="281" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X66">
-    <cfRule type="cellIs" dxfId="239" priority="278" operator="equal">
+    <cfRule type="cellIs" dxfId="218" priority="278" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="238" priority="279" operator="equal">
+    <cfRule type="cellIs" dxfId="217" priority="279" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ60">
-    <cfRule type="cellIs" dxfId="237" priority="276" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="216" priority="276" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ77:AJ89">
-    <cfRule type="cellIs" dxfId="236" priority="274" stopIfTrue="1" operator="notBetween">
+    <cfRule type="cellIs" dxfId="215" priority="274" stopIfTrue="1" operator="notBetween">
       <formula>-0.000001</formula>
       <formula>0.000001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="235" priority="275" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="214" priority="275" stopIfTrue="1" operator="between">
       <formula>-0.000001</formula>
       <formula>0.000001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ65">
-    <cfRule type="cellIs" dxfId="234" priority="277" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="213" priority="277" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ25:AJ27">
-    <cfRule type="cellIs" dxfId="233" priority="270" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="212" priority="270" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ76 AJ71:AJ72">
-    <cfRule type="cellIs" dxfId="232" priority="267" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="211" priority="267" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="231" priority="268" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="210" priority="268" stopIfTrue="1" operator="greaterThan">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="230" priority="269" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="209" priority="269" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ73:AJ75">
-    <cfRule type="cellIs" dxfId="229" priority="271" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="208" priority="271" stopIfTrue="1" operator="greaterThan">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="228" priority="272" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="207" priority="272" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="227" priority="273" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="206" priority="273" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ28">
-    <cfRule type="cellIs" dxfId="226" priority="266" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="205" priority="266" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ55">
-    <cfRule type="cellIs" dxfId="225" priority="265" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="204" priority="265" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ56:AJ57">
-    <cfRule type="cellIs" dxfId="224" priority="264" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="203" priority="264" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ44:AJ54">
-    <cfRule type="cellIs" dxfId="223" priority="263" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="202" priority="263" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ67">
-    <cfRule type="cellIs" dxfId="222" priority="261" operator="equal">
+    <cfRule type="cellIs" dxfId="201" priority="261" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="221" priority="262" operator="equal">
+    <cfRule type="cellIs" dxfId="200" priority="262" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ66">
-    <cfRule type="cellIs" dxfId="220" priority="259" operator="equal">
+    <cfRule type="cellIs" dxfId="199" priority="259" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="219" priority="260" operator="equal">
+    <cfRule type="cellIs" dxfId="198" priority="260" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M62">
-    <cfRule type="cellIs" dxfId="218" priority="258" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="197" priority="258" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BJ66">
-    <cfRule type="cellIs" dxfId="217" priority="257" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="196" priority="257" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BJ77:BJ89">
-    <cfRule type="cellIs" dxfId="216" priority="255" stopIfTrue="1" operator="notBetween">
+    <cfRule type="cellIs" dxfId="195" priority="255" stopIfTrue="1" operator="notBetween">
       <formula>-0.000001</formula>
       <formula>0.000001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="215" priority="256" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="194" priority="256" stopIfTrue="1" operator="between">
       <formula>-0.000001</formula>
       <formula>0.000001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BJ71:BJ72 BJ76">
-    <cfRule type="cellIs" dxfId="214" priority="249" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="193" priority="249" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="213" priority="250" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="192" priority="250" stopIfTrue="1" operator="greaterThan">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="212" priority="251" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="191" priority="251" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BJ73 BJ75">
-    <cfRule type="cellIs" dxfId="211" priority="252" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="190" priority="252" stopIfTrue="1" operator="greaterThan">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="210" priority="253" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="189" priority="253" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="209" priority="254" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="188" priority="254" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AW53:AW54">
-    <cfRule type="cellIs" dxfId="208" priority="241" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="187" priority="241" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W24:AK24 AM24:AS24 AM23:AY23">
-    <cfRule type="expression" dxfId="207" priority="244">
+    <cfRule type="expression" dxfId="186" priority="244">
       <formula>W$20&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AW59">
-    <cfRule type="cellIs" dxfId="206" priority="243" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="185" priority="243" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V68:AK68 AM68:AZ68 V20:AY20 V1:AY18">
-    <cfRule type="cellIs" dxfId="205" priority="238" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="184" priority="238" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="204" priority="239" operator="equal">
+    <cfRule type="cellIs" dxfId="183" priority="239" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD60">
-    <cfRule type="cellIs" dxfId="203" priority="233" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="182" priority="233" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD76 AD71:AD72">
-    <cfRule type="cellIs" dxfId="202" priority="228" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="181" priority="228" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="201" priority="229" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="180" priority="229" stopIfTrue="1" operator="greaterThan">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="200" priority="230" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="179" priority="230" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD77:AD89">
-    <cfRule type="cellIs" dxfId="199" priority="231" stopIfTrue="1" operator="notBetween">
+    <cfRule type="cellIs" dxfId="178" priority="231" stopIfTrue="1" operator="notBetween">
       <formula>-0.000001</formula>
       <formula>0.000001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="198" priority="232" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="177" priority="232" stopIfTrue="1" operator="between">
       <formula>-0.000001</formula>
       <formula>0.000001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD65">
-    <cfRule type="cellIs" dxfId="197" priority="234" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="176" priority="234" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD73:AD75">
-    <cfRule type="cellIs" dxfId="196" priority="235" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="175" priority="235" stopIfTrue="1" operator="greaterThan">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="195" priority="236" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="174" priority="236" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="194" priority="237" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="173" priority="237" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD44:AD54">
-    <cfRule type="cellIs" dxfId="193" priority="227" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="172" priority="227" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD66:AD67">
-    <cfRule type="cellIs" dxfId="192" priority="225" operator="equal">
+    <cfRule type="cellIs" dxfId="171" priority="225" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="191" priority="226" operator="equal">
+    <cfRule type="cellIs" dxfId="170" priority="226" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG60">
-    <cfRule type="cellIs" dxfId="190" priority="220" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="169" priority="220" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG71:AG72 AG76">
-    <cfRule type="cellIs" dxfId="189" priority="215" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="168" priority="215" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="188" priority="216" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="167" priority="216" stopIfTrue="1" operator="greaterThan">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="187" priority="217" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="166" priority="217" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG77:AG89">
-    <cfRule type="cellIs" dxfId="186" priority="218" stopIfTrue="1" operator="notBetween">
+    <cfRule type="cellIs" dxfId="165" priority="218" stopIfTrue="1" operator="notBetween">
       <formula>-0.000001</formula>
       <formula>0.000001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="185" priority="219" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="164" priority="219" stopIfTrue="1" operator="between">
       <formula>-0.000001</formula>
       <formula>0.000001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG65">
-    <cfRule type="cellIs" dxfId="184" priority="221" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="163" priority="221" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG73:AG75">
-    <cfRule type="cellIs" dxfId="183" priority="222" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="162" priority="222" stopIfTrue="1" operator="greaterThan">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="182" priority="223" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="161" priority="223" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="181" priority="224" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="160" priority="224" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG44:AG54">
-    <cfRule type="cellIs" dxfId="180" priority="214" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="159" priority="214" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG66:AG67">
-    <cfRule type="cellIs" dxfId="179" priority="212" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="212" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="178" priority="213" operator="equal">
+    <cfRule type="cellIs" dxfId="157" priority="213" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AT60">
-    <cfRule type="cellIs" dxfId="177" priority="210" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="156" priority="210" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AT59">
-    <cfRule type="cellIs" dxfId="176" priority="211" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="211" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AT61">
-    <cfRule type="cellIs" dxfId="175" priority="209" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="154" priority="209" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG66:AG67">
-    <cfRule type="cellIs" dxfId="174" priority="205" operator="equal">
+    <cfRule type="cellIs" dxfId="153" priority="205" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="173" priority="206" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="206" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU24:AY24">
-    <cfRule type="expression" dxfId="172" priority="204">
+    <cfRule type="expression" dxfId="151" priority="204">
       <formula>AU$20&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V68:AK68 AM68:AZ68">
-    <cfRule type="cellIs" dxfId="171" priority="203" operator="lessThan">
+    <cfRule type="cellIs" dxfId="150" priority="203" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AW69 Y69:AC69 AM69:AR69 AE69:AF69 AH69">
-    <cfRule type="cellIs" dxfId="170" priority="200" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="149" priority="200" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="169" priority="201" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="148" priority="201" stopIfTrue="1" operator="greaterThan">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="168" priority="202" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="147" priority="202" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI69 AS69">
-    <cfRule type="cellIs" dxfId="167" priority="197" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="146" priority="197" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="166" priority="198" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="145" priority="198" stopIfTrue="1" operator="greaterThan">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="165" priority="199" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="144" priority="199" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK69">
-    <cfRule type="cellIs" dxfId="164" priority="194" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="143" priority="194" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="163" priority="195" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="142" priority="195" stopIfTrue="1" operator="greaterThan">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="162" priority="196" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="141" priority="196" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AZ69">
-    <cfRule type="cellIs" dxfId="161" priority="191" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="140" priority="191" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="160" priority="192" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="139" priority="192" stopIfTrue="1" operator="greaterThan">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="159" priority="193" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="138" priority="193" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU69">
-    <cfRule type="cellIs" dxfId="158" priority="188" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="137" priority="188" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="157" priority="189" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="136" priority="189" stopIfTrue="1" operator="greaterThan">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="156" priority="190" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="135" priority="190" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AV69">
-    <cfRule type="cellIs" dxfId="155" priority="185" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="134" priority="185" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="154" priority="186" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="133" priority="186" stopIfTrue="1" operator="greaterThan">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="153" priority="187" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="132" priority="187" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AY69">
-    <cfRule type="cellIs" dxfId="152" priority="182" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="131" priority="182" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="151" priority="183" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="130" priority="183" stopIfTrue="1" operator="greaterThan">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="150" priority="184" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="129" priority="184" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AX69">
-    <cfRule type="cellIs" dxfId="149" priority="179" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="128" priority="179" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="148" priority="180" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="127" priority="180" stopIfTrue="1" operator="greaterThan">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="147" priority="181" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="126" priority="181" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AT69">
-    <cfRule type="cellIs" dxfId="146" priority="176" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="125" priority="176" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="145" priority="177" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="124" priority="177" stopIfTrue="1" operator="greaterThan">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="144" priority="178" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="123" priority="178" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V69">
-    <cfRule type="cellIs" dxfId="143" priority="173" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="122" priority="173" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="142" priority="174" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="121" priority="174" stopIfTrue="1" operator="greaterThan">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="141" priority="175" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="120" priority="175" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W69">
-    <cfRule type="cellIs" dxfId="140" priority="170" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="119" priority="170" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="139" priority="171" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="118" priority="171" stopIfTrue="1" operator="greaterThan">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="138" priority="172" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="117" priority="172" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X69">
-    <cfRule type="cellIs" dxfId="137" priority="167" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="116" priority="167" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="136" priority="168" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="115" priority="168" stopIfTrue="1" operator="greaterThan">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="135" priority="169" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="114" priority="169" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ69">
-    <cfRule type="cellIs" dxfId="134" priority="164" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="113" priority="164" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="133" priority="165" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="112" priority="165" stopIfTrue="1" operator="greaterThan">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="132" priority="166" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="111" priority="166" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD69">
-    <cfRule type="cellIs" dxfId="131" priority="161" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="110" priority="161" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="130" priority="162" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="109" priority="162" stopIfTrue="1" operator="greaterThan">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="129" priority="163" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="108" priority="163" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG69">
-    <cfRule type="cellIs" dxfId="128" priority="158" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="107" priority="158" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="127" priority="159" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="106" priority="159" stopIfTrue="1" operator="greaterThan">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="126" priority="160" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="105" priority="160" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V23:AK23">
-    <cfRule type="expression" dxfId="125" priority="157">
+    <cfRule type="expression" dxfId="104" priority="157">
       <formula>V$20&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL61:AL64 AL58:AL59 AL29:AL44">
-    <cfRule type="cellIs" dxfId="124" priority="152" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="152" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL66:AL67">
-    <cfRule type="cellIs" dxfId="123" priority="150" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="150" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL60">
-    <cfRule type="cellIs" dxfId="122" priority="151" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="151" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL56:AL57">
-    <cfRule type="cellIs" dxfId="121" priority="146" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="146" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL25:AL27 AL65">
-    <cfRule type="cellIs" dxfId="120" priority="149" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="149" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL28">
-    <cfRule type="cellIs" dxfId="119" priority="148" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="148" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL55">
-    <cfRule type="cellIs" dxfId="118" priority="147" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="147" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL45:AL54">
-    <cfRule type="cellIs" dxfId="117" priority="145" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="145" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL67">
-    <cfRule type="cellIs" dxfId="116" priority="143" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="143" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="115" priority="144" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="144" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL66">
-    <cfRule type="cellIs" dxfId="114" priority="141" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="141" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="113" priority="142" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="142" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL24">
-    <cfRule type="expression" dxfId="112" priority="140">
+    <cfRule type="expression" dxfId="91" priority="140">
       <formula>AL$20&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL68">
-    <cfRule type="cellIs" dxfId="111" priority="138" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="90" priority="138" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="110" priority="139" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="139" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL68">
-    <cfRule type="cellIs" dxfId="109" priority="137" operator="lessThan">
+    <cfRule type="cellIs" dxfId="88" priority="137" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL69">
-    <cfRule type="cellIs" dxfId="108" priority="134" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="87" priority="134" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="107" priority="135" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="86" priority="135" stopIfTrue="1" operator="greaterThan">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="106" priority="136" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="85" priority="136" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL23">
-    <cfRule type="expression" dxfId="105" priority="133">
+    <cfRule type="expression" dxfId="84" priority="133">
       <formula>AL$20&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL77:AL89">
-    <cfRule type="cellIs" dxfId="104" priority="131" stopIfTrue="1" operator="notBetween">
+    <cfRule type="cellIs" dxfId="83" priority="131" stopIfTrue="1" operator="notBetween">
       <formula>-0.000001</formula>
       <formula>0.000001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="103" priority="132" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="82" priority="132" stopIfTrue="1" operator="between">
       <formula>-0.000001</formula>
       <formula>0.000001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL76 AL71:AL72">
-    <cfRule type="cellIs" dxfId="102" priority="125" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="81" priority="125" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="126" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="80" priority="126" stopIfTrue="1" operator="greaterThan">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="127" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="79" priority="127" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL73:AL75">
-    <cfRule type="cellIs" dxfId="99" priority="128" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="78" priority="128" stopIfTrue="1" operator="greaterThan">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="129" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="77" priority="129" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="97" priority="130" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="76" priority="130" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AZ61:AZ64 AZ25:AZ58">
-    <cfRule type="cellIs" dxfId="96" priority="119" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="119" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AZ65">
-    <cfRule type="cellIs" dxfId="95" priority="118" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="118" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AZ59">
-    <cfRule type="cellIs" dxfId="94" priority="117" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="117" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AZ60">
-    <cfRule type="cellIs" dxfId="93" priority="116" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="116" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AW51:AW52">
-    <cfRule type="cellIs" dxfId="92" priority="115" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="115" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AX45">
-    <cfRule type="cellIs" dxfId="91" priority="114" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="114" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AX46">
-    <cfRule type="cellIs" dxfId="90" priority="112" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="112" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AY47">
-    <cfRule type="cellIs" dxfId="89" priority="111" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="111" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AY48">
-    <cfRule type="cellIs" dxfId="88" priority="110" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="110" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AY44">
-    <cfRule type="cellIs" dxfId="87" priority="109" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="109" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BD67:BD68">
-    <cfRule type="cellIs" dxfId="86" priority="103" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="65" priority="103" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="104" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="64" priority="104" stopIfTrue="1" operator="greaterThan">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="105" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="63" priority="105" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BJ61:BJ64 BJ25:BJ58">
-    <cfRule type="cellIs" dxfId="83" priority="100" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="100" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BJ60">
-    <cfRule type="cellIs" dxfId="82" priority="98" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="98" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BJ65">
-    <cfRule type="cellIs" dxfId="81" priority="99" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="99" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BJ59">
-    <cfRule type="cellIs" dxfId="80" priority="97" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="97" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BJ74">
-    <cfRule type="cellIs" dxfId="79" priority="94" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="58" priority="94" stopIfTrue="1" operator="greaterThan">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="95" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="57" priority="95" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="96" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="56" priority="96" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V66:AZ67">
-    <cfRule type="cellIs" dxfId="76" priority="92" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="55" priority="92" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="93" operator="lessThan">
+    <cfRule type="cellIs" dxfId="54" priority="93" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q27">
-    <cfRule type="cellIs" dxfId="74" priority="91" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="91" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI66">
-    <cfRule type="cellIs" dxfId="73" priority="89" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="89" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="90" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="90" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BA77">
-    <cfRule type="cellIs" dxfId="71" priority="86" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="50" priority="86" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="87" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="49" priority="87" stopIfTrue="1" operator="greaterThan">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="88" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="48" priority="88" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BL66 BL25:BL58 BL61:BL64">
-    <cfRule type="cellIs" dxfId="50" priority="22" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="22" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BL77:BL89">
-    <cfRule type="cellIs" dxfId="49" priority="20" stopIfTrue="1" operator="notBetween">
+    <cfRule type="cellIs" dxfId="46" priority="20" stopIfTrue="1" operator="notBetween">
       <formula>-0.000001</formula>
       <formula>0.000001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="21" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="45" priority="21" stopIfTrue="1" operator="between">
       <formula>-0.000001</formula>
       <formula>0.000001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BL71:BL72 BL76">
-    <cfRule type="cellIs" dxfId="47" priority="14" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="44" priority="14" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="15" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="43" priority="15" stopIfTrue="1" operator="greaterThan">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="16" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="42" priority="16" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BL73:BL75">
-    <cfRule type="cellIs" dxfId="44" priority="17" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="41" priority="17" stopIfTrue="1" operator="greaterThan">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="18" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="40" priority="18" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="19" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="39" priority="19" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BL60">
-    <cfRule type="cellIs" dxfId="41" priority="12" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="12" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BL65">
-    <cfRule type="cellIs" dxfId="40" priority="13" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="13" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BL69">
-    <cfRule type="cellIs" dxfId="39" priority="9" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="36" priority="9" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>-0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="10" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="35" priority="10" stopIfTrue="1" operator="greaterThan">
       <formula>0.00001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="11" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="34" priority="11" stopIfTrue="1" operator="between">
       <formula>-0.00001</formula>
       <formula>0.00001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BL59">
-    <cfRule type="cellIs" dxfId="36" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="8" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -44713,9 +44476,7 @@
   </sheetPr>
   <dimension ref="A1:AA17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>